<commit_message>
Few small fixes to IO notebook
</commit_message>
<xml_diff>
--- a/Day 1 PM/files/excel_importer_example.xlsx
+++ b/Day 1 PM/files/excel_importer_example.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mypy\MyNotebooks\Brightway-Seminar-2017\Day 1 PM\files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1284" yWindow="0" windowWidth="28296" windowHeight="20520" activeTab="1"/>
+    <workbookView xWindow="1280" yWindow="0" windowWidth="28300" windowHeight="20520" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="skip this sheet" sheetId="2" r:id="rId1"/>
     <sheet name="first process" sheetId="1" r:id="rId2"/>
     <sheet name="other process" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="60">
   <si>
     <t>Database</t>
   </si>
@@ -203,12 +198,15 @@
   </si>
   <si>
     <t>WriteSomeCode_UUID_isFineButNotNecessary</t>
+  </si>
+  <si>
+    <t>ecoinvent 2.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -266,8 +264,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -287,17 +287,19 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -604,24 +606,24 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
@@ -641,10 +643,10 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="50.6640625" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" customWidth="1"/>
@@ -655,7 +657,7 @@
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -666,7 +668,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -677,7 +679,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -688,12 +690,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="15">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -704,7 +706,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -712,7 +714,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -720,7 +722,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -728,7 +730,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -736,7 +738,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -744,7 +746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -752,7 +754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -760,12 +762,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="15">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -803,7 +805,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -814,7 +816,7 @@
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
         <v>47</v>
@@ -841,7 +843,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -852,7 +854,7 @@
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="E17" t="s">
         <v>46</v>
@@ -879,7 +881,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -919,7 +921,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -936,9 +938,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -946,12 +948,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="15">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -959,7 +961,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -967,7 +969,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -975,7 +977,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -983,7 +985,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -991,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -999,7 +1001,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1016,7 +1018,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="15">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1030,7 +1032,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="15">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -1068,7 +1070,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1110,7 +1112,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -1148,7 +1150,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
Add corrected importer examples files
</commit_message>
<xml_diff>
--- a/Day 1 PM/files/excel_importer_example.xlsx
+++ b/Day 1 PM/files/excel_importer_example.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="59">
   <si>
     <t>Database</t>
   </si>
@@ -165,9 +165,6 @@
   </si>
   <si>
     <t>CH</t>
-  </si>
-  <si>
-    <t>water bottle</t>
   </si>
   <si>
     <t>water bottle production</t>
@@ -207,9 +204,23 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -264,42 +275,76 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -643,7 +688,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -700,7 +745,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>31</v>
@@ -759,7 +804,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15">
@@ -816,10 +861,10 @@
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F16" t="s">
         <v>25</v>
@@ -854,7 +899,7 @@
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
         <v>46</v>
@@ -881,8 +926,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
-      <c r="A18" t="s">
+    <row r="18" spans="1:12" ht="15">
+      <c r="A18" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B18">
@@ -891,11 +936,11 @@
       <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D18" t="s">
-        <v>27</v>
+      <c r="D18" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F18" t="s">
         <v>24</v>
@@ -935,10 +980,13 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="41.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
@@ -958,7 +1006,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -974,7 +1022,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1006,16 +1054,16 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="O10" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="P10">
         <v>200</v>
       </c>
       <c r="Q10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="15">
@@ -1023,13 +1071,13 @@
         <v>13</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P11">
         <v>1</v>
       </c>
       <c r="Q11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="15">
@@ -1070,8 +1118,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
-      <c r="A13" t="s">
+    <row r="13" spans="1:17" ht="15">
+      <c r="A13" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B13">
@@ -1085,7 +1133,7 @@
         <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F13" t="s">
         <v>25</v>
@@ -1114,16 +1162,16 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
         <v>47</v>
@@ -1152,16 +1200,16 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
         <v>47</v>
@@ -1190,6 +1238,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>